<commit_message>
feat:new name plate data
</commit_message>
<xml_diff>
--- a/NamePlateTransData.xlsx
+++ b/NamePlateTransData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeNamePlate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B0D9B-7211-40F7-B872-473A5C3214BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D19809-C91D-4634-8D1C-7FFEC0A591F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>English</t>
   </si>
@@ -117,6 +117,65 @@
     <rPh sb="8" eb="9">
       <t>アオ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>developerRed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開発者の証 - 赤</t>
+    <rPh sb="0" eb="3">
+      <t>カイハツシャ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>アカシ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>アカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スターフィールド - 銀河</t>
+    <rPh sb="11" eb="13">
+      <t>ギンガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>starFieldGalaxy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>starFieldNebura</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スターフィールド - 星雲</t>
+    <rPh sb="11" eb="13">
+      <t>セイウン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>extremeRolesLogo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>extremeSkinsLogo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ロゴ - Extreme Roles</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ロゴ - Extreme Skins</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -448,7 +507,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -535,6 +594,49 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
     </row>

</xml_diff>

<commit_message>
feat:v3.2.0.0NamePlate.Thunk you クロドル, アンハッピーセット
</commit_message>
<xml_diff>
--- a/NamePlateTransData.xlsx
+++ b/NamePlateTransData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895415C2-BFAD-4999-ADF2-F1C9BF9464CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975EAE5C-B7E7-4CBB-B50C-369D2F7AE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>English</t>
   </si>
@@ -203,6 +203,47 @@
   </si>
   <si>
     <t>SW-Needle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>minicrewmate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ミニクルーメイト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ligftdown</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ライトダウン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CAT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>猫(青)</t>
+    <rPh sb="0" eb="1">
+      <t>ネコ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gentle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>紳士</t>
+    <rPh sb="0" eb="2">
+      <t>シンシ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -533,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -699,13 +740,45 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.4">

</xml_diff>